<commit_message>
Added power supply and analog front ends for sensor
</commit_message>
<xml_diff>
--- a/mechanical/TestEngine1/BOM.xlsx
+++ b/mechanical/TestEngine1/BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roy\Documents\GitHub\LaunchInitiative\Rocket_test_1\Engine\Solidworks Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roy\Documents\GitHub\RITLaunchInitiative\mechanical\TestEngine1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Nylon bushing</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>quantity</t>
+  </si>
+  <si>
+    <t>High Temp O ring</t>
+  </si>
+  <si>
+    <t>9396K115</t>
   </si>
 </sst>
 </file>
@@ -74,7 +80,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -82,13 +88,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,32 +391,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:G4"/>
+  <dimension ref="C3:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
     <col min="4" max="4" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -404,6 +426,14 @@
       </c>
       <c r="D4" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>